<commit_message>
Regression test execution 20221109
</commit_message>
<xml_diff>
--- a/doc/regression-test/suites/legacy-security/03-credential.xlsx
+++ b/doc/regression-test/suites/legacy-security/03-credential.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\Dev\Propel\propel\doc\regression-test\suites\legacy-security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13DC23A-5BAF-45DE-9BB9-551AC13FFEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE91B6-A72D-4C32-A834-36B55689B6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="156">
   <si>
     <t>Description</t>
   </si>
@@ -221,9 +221,6 @@
 Field Name: FieldAWS01
 Field Value: AWS Value
 Then click on the Save button</t>
-  </si>
-  <si>
-    <t>"Touch" (click) over eash one of the form fields.</t>
   </si>
   <si>
     <t>For all the fields with the red exclamation point you will see a legend below indicating the field value is required</t>
@@ -750,6 +747,9 @@
   </si>
   <si>
     <t>03_TargetCredential</t>
+  </si>
+  <si>
+    <t>"Touch" (click) over each one of the form fields.</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1050,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1130,14 +1130,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="111">
+  <dxfs count="72">
     <dxf>
       <font>
         <b val="0"/>
@@ -1223,19 +1220,10 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
-        <color auto="1"/>
+        <strike val="0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1319,10 +1307,19 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
-        <strike val="0"/>
+        <color auto="1"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1344,50 +1341,6 @@
       <font>
         <b/>
         <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
       </font>
     </dxf>
@@ -1481,43 +1434,9 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFF1826F"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1529,130 +1448,6 @@
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1925,13 +1720,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FFBFBFBF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color rgb="FFA6A6A6"/>
         </top>
@@ -1966,6 +1754,13 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FFBFBFBF"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1989,209 +1784,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1826F"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2442,13 +2034,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FFBFBFBF"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color rgb="FFA6A6A6"/>
         </top>
@@ -2481,6 +2066,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FFBFBFBF"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3997,11 +3589,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}" name="Summary" displayName="Summary" ref="A1:B4" totalsRowShown="0" headerRowDxfId="110" headerRowBorderDxfId="109" tableBorderDxfId="108" totalsRowBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}" name="Summary" displayName="Summary" ref="A1:B4" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
   <autoFilter ref="A1:B4" xr:uid="{4408209C-EE48-4EDD-81CA-828422C6913B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{654C6343-7B3C-42FE-9EF4-7BFE7BE35779}" name="Test Case Sheet name" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{FDA0E746-B4F2-405E-8A1D-9A6A22073CB9}" name="Result" dataDxfId="105">
+    <tableColumn id="1" xr3:uid="{654C6343-7B3C-42FE-9EF4-7BFE7BE35779}" name="Test Case Sheet name" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{FDA0E746-B4F2-405E-8A1D-9A6A22073CB9}" name="Result" dataDxfId="66">
       <calculatedColumnFormula array="1">INDIRECT(A2&amp;"!E8")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4010,21 +3602,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}" name="SummaryResults" displayName="SummaryResults" ref="D1:E4" totalsRowShown="0" headerRowDxfId="104" headerRowBorderDxfId="103" tableBorderDxfId="102" totalsRowBorderDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}" name="SummaryResults" displayName="SummaryResults" ref="D1:E4" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64" tableBorderDxfId="63" totalsRowBorderDxfId="62">
   <autoFilter ref="D1:E4" xr:uid="{949BDB15-3C75-449C-B4C4-A2C0E485B5C0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5420B28C-70A3-47FD-BF8A-F016E4F7FA0F}" name="Summary Results" dataDxfId="100"/>
-    <tableColumn id="2" xr3:uid="{B0E66881-1E02-43BC-AA03-3C33769D1162}" name="Count" dataDxfId="99"/>
+    <tableColumn id="1" xr3:uid="{5420B28C-70A3-47FD-BF8A-F016E4F7FA0F}" name="Summary Results" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{B0E66881-1E02-43BC-AA03-3C33769D1162}" name="Count" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D3E09E6-43C8-4788-BA0E-09F9C445D7D5}" name="SampleTestCase12" displayName="SampleTestCase12" ref="A10:F34" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D3E09E6-43C8-4788-BA0E-09F9C445D7D5}" name="SampleTestCase12" displayName="SampleTestCase12" ref="A10:F34" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <autoFilter ref="A10:F34" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4034,22 +3626,22 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{28386F51-EA89-4E22-94FE-E643A1522C73}" name="Step#" dataDxfId="93">
+    <tableColumn id="1" xr3:uid="{28386F51-EA89-4E22-94FE-E643A1522C73}" name="Step#" dataDxfId="54">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AD88C9C6-DADE-45D0-A01C-3DD953458433}" name="Area" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{B02D9B2C-E852-4462-A564-81E53B5B365B}" name="Step Details" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{CDFDD06A-E36F-4E48-8FBC-00C2BA7A82BE}" name="Expected" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{6A3BB6D8-A91E-4A24-9EE4-7F664D029AC6}" name="Actual" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{965FEC3D-F8DD-479C-99AA-27E03D4F4B08}" name="Status" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{AD88C9C6-DADE-45D0-A01C-3DD953458433}" name="Area" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{B02D9B2C-E852-4462-A564-81E53B5B365B}" name="Step Details" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{CDFDD06A-E36F-4E48-8FBC-00C2BA7A82BE}" name="Expected" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{6A3BB6D8-A91E-4A24-9EE4-7F664D029AC6}" name="Actual" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{965FEC3D-F8DD-479C-99AA-27E03D4F4B08}" name="Status" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F56471D-DB83-48A9-B9AB-11C3A8E920ED}" name="SampleTestCase123" displayName="SampleTestCase123" ref="A10:F44" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86" headerRowBorderDxfId="84" tableBorderDxfId="85" totalsRowBorderDxfId="83">
-  <autoFilter ref="A10:F44" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F56471D-DB83-48A9-B9AB-11C3A8E920ED}" name="SampleTestCase123" displayName="SampleTestCase123" ref="A10:F43" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="A10:F43" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -4058,21 +3650,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{530E2121-750A-45CF-AF54-3ACDD528C367}" name="Step#" dataDxfId="82">
+    <tableColumn id="1" xr3:uid="{530E2121-750A-45CF-AF54-3ACDD528C367}" name="Step#" dataDxfId="43">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{51E1B407-15FB-4927-AAAF-421C560575E1}" name="Area" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{114C6BD4-8687-418A-8C55-D6188420ED6F}" name="Step Details" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{541070CC-275D-4C84-AF4F-023A6949B6ED}" name="Expected" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{7EEEF59A-F3B5-43A1-8566-E7C4E5341B42}" name="Actual" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{3784143B-3686-44E8-BA0C-9E882F3D303B}" name="Status" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{51E1B407-15FB-4927-AAAF-421C560575E1}" name="Area" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{114C6BD4-8687-418A-8C55-D6188420ED6F}" name="Step Details" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{541070CC-275D-4C84-AF4F-023A6949B6ED}" name="Expected" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{7EEEF59A-F3B5-43A1-8566-E7C4E5341B42}" name="Actual" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{3784143B-3686-44E8-BA0C-9E882F3D303B}" name="Status" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A174960A-04F0-4654-8495-D3DAAEB72DF9}" name="SampleTestCase1236" displayName="SampleTestCase1236" ref="A10:F23" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" headerRowBorderDxfId="52" tableBorderDxfId="53" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A174960A-04F0-4654-8495-D3DAAEB72DF9}" name="SampleTestCase1236" displayName="SampleTestCase1236" ref="A10:F23" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A10:F23" xr:uid="{5E4571F6-B23A-41AD-A10C-A2AD2284AD4B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4082,14 +3674,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0C88C63F-5489-4D9B-8F14-2B1375C56DF7}" name="Step#" dataDxfId="50">
+    <tableColumn id="1" xr3:uid="{0C88C63F-5489-4D9B-8F14-2B1375C56DF7}" name="Step#" dataDxfId="32">
       <calculatedColumnFormula>IF(ISNUMBER(A10), A10 +1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{2BEAB6A4-8E0B-451F-B090-BA5F2556688B}" name="Area" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{D0259EF1-21BD-4580-978F-A1F7EEB3A024}" name="Step Details" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{9A46C078-27AE-4C04-B971-97C7194BDCDC}" name="Expected" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{19DAAB18-8EE8-4E31-9892-B29CAD04B1AE}" name="Actual" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{09F21995-B2DE-4744-BA42-470C3FE66205}" name="Status" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{2BEAB6A4-8E0B-451F-B090-BA5F2556688B}" name="Area" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{D0259EF1-21BD-4580-978F-A1F7EEB3A024}" name="Step Details" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{9A46C078-27AE-4C04-B971-97C7194BDCDC}" name="Expected" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{19DAAB18-8EE8-4E31-9892-B29CAD04B1AE}" name="Actual" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{09F21995-B2DE-4744-BA42-470C3FE66205}" name="Status" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4389,7 +3981,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">INDIRECT(A2&amp;"!E8")</f>
@@ -4405,7 +3997,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">INDIRECT(A3&amp;"!E8")</f>
@@ -4421,7 +4013,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B4" s="9" t="str" cm="1">
         <f t="array" aca="1" ref="B4" ca="1">INDIRECT(A4&amp;"!E8")</f>
@@ -4451,8 +4043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D215E9-B302-441A-A0B0-4EC6D3FC68F0}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4475,7 +4067,7 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -4498,10 +4090,10 @@
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>143</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
@@ -4509,7 +4101,7 @@
       </c>
       <c r="E5" s="5">
         <f>COUNTIF(SampleTestCase12[Status], "Not Executed")</f>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F5" s="15">
         <f>E5/SUM(E$5:E$7)</f>
@@ -4614,7 +4206,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
@@ -4630,10 +4222,10 @@
         <v>33</v>
       </c>
       <c r="C13" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="4" t="s">
@@ -4649,10 +4241,10 @@
         <v>33</v>
       </c>
       <c r="C14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
@@ -4668,10 +4260,10 @@
         <v>33</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="4" t="s">
@@ -4766,7 +4358,7 @@
         <v>35</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="4" t="s">
@@ -4782,10 +4374,10 @@
         <v>34</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
@@ -4855,13 +4447,13 @@
         <v>15</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>46</v>
-      </c>
       <c r="D25" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
@@ -4874,13 +4466,13 @@
         <v>16</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
@@ -4893,10 +4485,10 @@
         <v>17</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>27</v>
@@ -4912,10 +4504,10 @@
         <v>18</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>28</v>
@@ -4931,7 +4523,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>31</v>
@@ -4950,16 +4542,18 @@
         <v>20</v>
       </c>
       <c r="B30" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>147</v>
-      </c>
       <c r="E30" s="21"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
@@ -4967,16 +4561,18 @@
         <v>21</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C31" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>149</v>
-      </c>
       <c r="E31" s="21"/>
-      <c r="F31" s="27"/>
+      <c r="F31" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
@@ -4984,16 +4580,18 @@
         <v>22</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C32" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>151</v>
-      </c>
       <c r="E32" s="21"/>
-      <c r="F32" s="27"/>
+      <c r="F32" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
@@ -5001,16 +4599,18 @@
         <v>23</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E33" s="21"/>
-      <c r="F33" s="27"/>
+      <c r="F33" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="247" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
@@ -5018,16 +4618,18 @@
         <v>24</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C34" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>154</v>
-      </c>
       <c r="E34" s="21"/>
-      <c r="F34" s="27"/>
+      <c r="F34" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5040,28 +4642,28 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="F11:F34">
-    <cfRule type="expression" dxfId="24" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>$F11="Fail"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>$F11="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>$E$8="Pass"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="23" priority="3">
       <formula>$E$8="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:F34">
-    <cfRule type="expression" dxfId="20" priority="7">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B34">
-    <cfRule type="expression" dxfId="19" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5080,10 +4682,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA94D0F-DC5D-4922-9534-E4D1087EA20D}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5106,7 +4708,7 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -5129,10 +4731,10 @@
     </row>
     <row r="5" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>61</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
@@ -5140,7 +4742,7 @@
       </c>
       <c r="E5" s="5">
         <f>COUNTIF(SampleTestCase123[Status], "Not Executed")</f>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="15">
         <f>E5/SUM(E$5:E$7)</f>
@@ -5216,11 +4818,11 @@
     </row>
     <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
-        <f t="shared" ref="A11:A44" si="1">IF(ISNUMBER(A10), A10 +1, 1)</f>
+        <f t="shared" ref="A11:A43" si="1">IF(ISNUMBER(A10), A10 +1, 1)</f>
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>20</v>
@@ -5239,13 +4841,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
@@ -5258,186 +4860,186 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>64</v>
+        <v>78</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="17"/>
+        <v>66</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="156" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="10" t="s">
         <v>67</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="156" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
-        <f t="shared" si="1"/>
+        <f>IF(ISNUMBER(A19), A19 +1, 1)</f>
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>71</v>
+        <v>78</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="10"/>
+        <v>73</v>
+      </c>
+      <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="D21" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="10"/>
       <c r="F21" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
         <v>6</v>
       </c>
@@ -5448,13 +5050,13 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>76</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
@@ -5470,83 +5072,83 @@
         <v>79</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="143" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="143" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>32</v>
+        <v>55</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="17"/>
+        <v>82</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="21"/>
       <c r="F27" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>86</v>
@@ -5556,35 +5158,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>88</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="195" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>90</v>
@@ -5594,57 +5196,57 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="195" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="117" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>92</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="117" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="78" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E32" s="21"/>
       <c r="F32" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="78" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E33" s="21"/>
       <c r="F33" s="4" t="s">
@@ -5657,7 +5259,7 @@
         <v>24</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>97</v>
@@ -5670,149 +5272,149 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D36" s="20" t="s">
         <v>102</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>103</v>
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="130" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="10" t="s">
         <v>104</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="E37" s="21"/>
       <c r="F37" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="130" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E38" s="21"/>
       <c r="F38" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="52" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E39" s="21"/>
       <c r="F39" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="52" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="130" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E40" s="21"/>
       <c r="F40" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="130" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E41" s="21"/>
       <c r="F41" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>99</v>
@@ -5822,41 +5424,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="E43" s="21"/>
       <c r="F43" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A44" s="5">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="E44" s="21"/>
-      <c r="F44" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5869,64 +5452,74 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
   </mergeCells>
-  <conditionalFormatting sqref="F11:F44">
-    <cfRule type="expression" dxfId="18" priority="9">
+  <conditionalFormatting sqref="F11:F43">
+    <cfRule type="expression" dxfId="20" priority="9">
       <formula>$F11="Fail"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="10">
+    <cfRule type="expression" dxfId="19" priority="10">
       <formula>$F11="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="18" priority="7">
       <formula>$E$8="Pass"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="8">
+    <cfRule type="expression" dxfId="17" priority="8">
       <formula>$E$8="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:F11 B17:C17 E17:F17 B18:F21 B22:C22 E22:F22 B23:F25 B12:B24 B26:C26 E26:F26 B27:F29 B12:F16 A12:A44 F30:F44">
-    <cfRule type="expression" dxfId="14" priority="12">
+  <conditionalFormatting sqref="B16:C16 E16:F16 B21:C21 E21:F21 B22:F24 B25:C25 E25:F25 B26:F28 F29:F43 B14:F15 A11:F11 B12:F12 B21:B23 A21:A43 A12:A19 B14:B19 B17:F19 A20:F20">
+    <cfRule type="expression" dxfId="16" priority="12">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B44">
-    <cfRule type="expression" dxfId="13" priority="11">
+  <conditionalFormatting sqref="B11:B12 B14:B43">
+    <cfRule type="expression" dxfId="15" priority="11">
       <formula>AND($B11&lt;&gt;$B10)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="12" priority="6">
-      <formula>AND($B17&lt;&gt;$B16)</formula>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="14" priority="6">
+      <formula>AND($B16&lt;&gt;$B15)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="11" priority="5">
-      <formula>AND($B22&lt;&gt;$B21)</formula>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="13" priority="5">
+      <formula>AND($B21&lt;&gt;$B20)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>AND($B26&lt;&gt;$B25)</formula>
+  <conditionalFormatting sqref="D25">
+    <cfRule type="expression" dxfId="12" priority="4">
+      <formula>AND($B25&lt;&gt;$B24)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B44">
-    <cfRule type="expression" dxfId="9" priority="3">
-      <formula>AND($B30&lt;&gt;$B29)</formula>
+  <conditionalFormatting sqref="B29:B43">
+    <cfRule type="expression" dxfId="11" priority="3">
+      <formula>AND($B29&lt;&gt;$B28)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>AND($B34&lt;&gt;$B33)</formula>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>AND($B33&lt;&gt;$B32)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>AND($B37&lt;&gt;$B36)</formula>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>AND($B36&lt;&gt;$B35)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:F13">
+    <cfRule type="expression" dxfId="8" priority="18">
+      <formula>AND($B13&lt;&gt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="expression" dxfId="7" priority="27">
+      <formula>AND($B13&lt;&gt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F44" xr:uid="{FC98A731-1400-4E99-A9D1-AB3F69DF5B22}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F43" xr:uid="{FC98A731-1400-4E99-A9D1-AB3F69DF5B22}">
       <formula1>"Pass,Fail,Not Executed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5942,8 +5535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94318C6C-E595-41D9-8AC8-D59514AA9452}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5966,7 +5559,7 @@
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -5989,10 +5582,10 @@
     </row>
     <row r="5" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>58</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>59</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="1" t="s">
@@ -6012,7 +5605,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="1" t="s">
@@ -6084,7 +5677,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>20</v>
@@ -6103,13 +5696,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>121</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
@@ -6122,13 +5715,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="4" t="s">
@@ -6141,13 +5734,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
@@ -6160,13 +5753,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="4" t="s">
@@ -6179,13 +5772,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>127</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
@@ -6198,13 +5791,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>131</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
@@ -6217,13 +5810,13 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
@@ -6236,13 +5829,13 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>135</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="4" t="s">
@@ -6255,13 +5848,13 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="4" t="s">
@@ -6274,13 +5867,13 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C21" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>137</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>138</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
@@ -6293,13 +5886,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="4" t="s">
@@ -6312,13 +5905,13 @@
         <v>13</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>141</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">

</xml_diff>